<commit_message>
Finish Carly, George, James, and Lawrence!
</commit_message>
<xml_diff>
--- a/data/GoodCSVs/BobbyJindal.xlsx
+++ b/data/GoodCSVs/BobbyJindal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>AL</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>March_16</t>
   </si>
 </sst>
 </file>
@@ -1054,16 +1057,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N11" sqref="N11"/>
+      <selection pane="topRight" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="9.140625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -1097,11 +1103,14 @@
       <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1135,11 +1144,14 @@
       <c r="K2" s="6">
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
         <v>2759</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1173,11 +1185,14 @@
       <c r="K3" s="6">
         <v>0</v>
       </c>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1211,11 +1226,14 @@
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
         <v>8925</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1249,11 +1267,14 @@
       <c r="K5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
         <v>3950</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1287,11 +1308,14 @@
       <c r="K6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
         <v>23231.26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1325,11 +1349,14 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
         <v>7000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1363,11 +1390,14 @@
       <c r="K8" s="6">
         <v>0</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
         <v>2700</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1401,11 +1431,14 @@
       <c r="K9" s="6">
         <v>0</v>
       </c>
-      <c r="L9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -1439,11 +1472,14 @@
       <c r="K10" s="6">
         <v>0</v>
       </c>
-      <c r="L10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1477,11 +1513,14 @@
       <c r="K11" s="6">
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
         <v>32050</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1515,11 +1554,14 @@
       <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
         <v>3600</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -1553,11 +1595,14 @@
       <c r="K13" s="6">
         <v>0</v>
       </c>
-      <c r="L13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1591,11 +1636,14 @@
       <c r="K14" s="6">
         <v>0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
         <v>1050</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1629,11 +1677,14 @@
       <c r="K15" s="6">
         <v>0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
         <v>5500</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1667,11 +1718,14 @@
       <c r="K16" s="6">
         <v>0</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
         <v>3450</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1705,11 +1759,14 @@
       <c r="K17" s="6">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
         <v>6420.16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1743,11 +1800,14 @@
       <c r="K18" s="6">
         <v>0</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="6">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -1781,11 +1841,14 @@
       <c r="K19" s="6">
         <v>0</v>
       </c>
-      <c r="L19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" s="6">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
@@ -1819,11 +1882,14 @@
       <c r="K20" s="6">
         <v>0</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
         <v>934939.32</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
@@ -1857,11 +1923,14 @@
       <c r="K21" s="6">
         <v>0</v>
       </c>
-      <c r="L21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -1895,11 +1964,14 @@
       <c r="K22" s="6">
         <v>0</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
         <v>9650</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1933,11 +2005,14 @@
       <c r="K23" s="6">
         <v>0</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="6">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -1971,11 +2046,14 @@
       <c r="K24" s="6">
         <v>0</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="6">
+        <v>0</v>
+      </c>
+      <c r="M24" s="4">
         <v>11300</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
@@ -2009,11 +2087,14 @@
       <c r="K25" s="6">
         <v>0</v>
       </c>
-      <c r="L25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="6">
+        <v>0</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -2047,11 +2128,14 @@
       <c r="K26" s="6">
         <v>0</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="6">
+        <v>0</v>
+      </c>
+      <c r="M26" s="4">
         <v>13500</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -2085,11 +2169,14 @@
       <c r="K27" s="6">
         <v>0</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="6">
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
         <v>12060</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>57</v>
       </c>
@@ -2123,11 +2210,14 @@
       <c r="K28" s="6">
         <v>0</v>
       </c>
-      <c r="L28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="6">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
@@ -2161,11 +2251,14 @@
       <c r="K29" s="6">
         <v>0</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="6">
+        <v>0</v>
+      </c>
+      <c r="M29" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
@@ -2199,11 +2292,14 @@
       <c r="K30" s="6">
         <v>0</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="6">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -2237,11 +2333,14 @@
       <c r="K31" s="6">
         <v>0</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="6">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4">
         <v>1250</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
@@ -2275,11 +2374,14 @@
       <c r="K32" s="6">
         <v>0</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="6">
+        <v>0</v>
+      </c>
+      <c r="M32" s="4">
         <v>6250</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
@@ -2313,11 +2415,14 @@
       <c r="K33" s="6">
         <v>0</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="6">
+        <v>0</v>
+      </c>
+      <c r="M33" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
@@ -2351,11 +2456,14 @@
       <c r="K34" s="6">
         <v>0</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="6">
+        <v>0</v>
+      </c>
+      <c r="M34" s="4">
         <v>32176.42</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>19</v>
       </c>
@@ -2389,11 +2497,14 @@
       <c r="K35" s="6">
         <v>0</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="6">
+        <v>0</v>
+      </c>
+      <c r="M35" s="4">
         <v>15885</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>58</v>
       </c>
@@ -2427,11 +2538,14 @@
       <c r="K36" s="6">
         <v>0</v>
       </c>
-      <c r="L36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="6">
+        <v>0</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>26</v>
       </c>
@@ -2465,11 +2579,14 @@
       <c r="K37" s="6">
         <v>0</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="6">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4">
         <v>3420.16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>27</v>
       </c>
@@ -2503,11 +2620,14 @@
       <c r="K38" s="6">
         <v>0</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="6">
+        <v>0</v>
+      </c>
+      <c r="M38" s="4">
         <v>7143</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>28</v>
       </c>
@@ -2541,11 +2661,14 @@
       <c r="K39" s="6">
         <v>0</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="6">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4">
         <v>270.16000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>29</v>
       </c>
@@ -2579,11 +2702,14 @@
       <c r="K40" s="6">
         <v>0</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="6">
+        <v>0</v>
+      </c>
+      <c r="M40" s="4">
         <v>7595.16</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
@@ -2617,11 +2743,14 @@
       <c r="K41" s="6">
         <v>0</v>
       </c>
-      <c r="L41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L41" s="6">
+        <v>0</v>
+      </c>
+      <c r="M41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
@@ -2655,11 +2784,14 @@
       <c r="K42" s="6">
         <v>0</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="6">
+        <v>0</v>
+      </c>
+      <c r="M42" s="4">
         <v>2061.2600000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>31</v>
       </c>
@@ -2693,11 +2825,14 @@
       <c r="K43" s="6">
         <v>0</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="6">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>32</v>
       </c>
@@ -2731,11 +2866,14 @@
       <c r="K44" s="6">
         <v>0</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="6">
+        <v>0</v>
+      </c>
+      <c r="M44" s="4">
         <v>1050</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>33</v>
       </c>
@@ -2769,11 +2907,14 @@
       <c r="K45" s="6">
         <v>0</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="6">
+        <v>0</v>
+      </c>
+      <c r="M45" s="4">
         <v>45160</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>34</v>
       </c>
@@ -2807,11 +2948,14 @@
       <c r="K46" s="6">
         <v>0</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="6">
+        <v>0</v>
+      </c>
+      <c r="M46" s="4">
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -2848,8 +2992,11 @@
       <c r="L47" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>35</v>
       </c>
@@ -2883,11 +3030,14 @@
       <c r="K48" s="6">
         <v>0</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="6">
+        <v>0</v>
+      </c>
+      <c r="M48" s="4">
         <v>19716</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>36</v>
       </c>
@@ -2921,11 +3071,14 @@
       <c r="K49" s="6">
         <v>0</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="6">
+        <v>0</v>
+      </c>
+      <c r="M49" s="4">
         <v>6231.26</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
@@ -2962,8 +3115,11 @@
       <c r="L50" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>37</v>
       </c>
@@ -2997,11 +3153,14 @@
       <c r="K51" s="6">
         <v>0</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51" s="6">
+        <v>0</v>
+      </c>
+      <c r="M51" s="4">
         <v>32000</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>62</v>
       </c>
@@ -3038,8 +3197,11 @@
       <c r="L52" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -3049,7 +3211,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>